<commit_message>
Add IO for a relay board
</commit_message>
<xml_diff>
--- a/Rev2_F401RE/eagle/revb_BOM_assembly.xlsx
+++ b/Rev2_F401RE/eagle/revb_BOM_assembly.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wpi0-my.sharepoint.com/personal/jwbuchta_wpi_edu/Documents/Projects/Interrupter/TeslaCoilController/Rev2_F401RE/eagle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="8_{6E2CAA61-36B4-4ECB-9F70-2D9154124FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FE95BFA-863E-4F80-AD1B-8939B0A6826D}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="8_{6E2CAA61-36B4-4ECB-9F70-2D9154124FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7DA6A34-9456-48BA-8326-475C243DB6F0}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{D47F748F-FF22-4AD5-A6FA-A0F321CBB47E}"/>
+    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="9984" xr2:uid="{D47F748F-FF22-4AD5-A6FA-A0F321CBB47E}"/>
   </bookViews>
   <sheets>
     <sheet name="revb_BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>Qty</t>
   </si>
@@ -58,24 +58,9 @@
     <t>L1, L2</t>
   </si>
   <si>
-    <t>MCP73832</t>
-  </si>
-  <si>
-    <t>SOT95P280X145-5N</t>
-  </si>
-  <si>
-    <t>IC2</t>
-  </si>
-  <si>
-    <t>Charge Management Controller</t>
-  </si>
-  <si>
     <t>J2</t>
   </si>
   <si>
-    <t>MMBTA06-7-F</t>
-  </si>
-  <si>
     <t>SOT23-BEC</t>
   </si>
   <si>
@@ -85,12 +70,6 @@
     <t>NPN Transistor</t>
   </si>
   <si>
-    <t>SI7615</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
     <t>STM32F401RE</t>
   </si>
   <si>
@@ -112,89 +91,101 @@
     <t>IC5</t>
   </si>
   <si>
-    <t>USB4105-GF-A</t>
-  </si>
-  <si>
-    <t>GCT_USB4105-GF-A</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>USBLC6-2SC6</t>
-  </si>
-  <si>
-    <t>SOT95P280X145-6N</t>
-  </si>
-  <si>
-    <t>D100</t>
-  </si>
-  <si>
     <t>Designator</t>
   </si>
   <si>
     <t>Value / PN</t>
   </si>
   <si>
-    <t>R115, R128, R130, R132, R134, R136, R138, R139, R142, R144, 
+    <t xml:space="preserve">Inductor </t>
+  </si>
+  <si>
+    <t>Microcontroller</t>
+  </si>
+  <si>
+    <t>5V regulator</t>
+  </si>
+  <si>
+    <t>3.3V regulator</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>10VSON</t>
+  </si>
+  <si>
+    <t>CAPACITOR</t>
+  </si>
+  <si>
+    <t>RESISTOR</t>
+  </si>
+  <si>
+    <t>Micro SD Card connector</t>
+  </si>
+  <si>
+    <t>C201, C204, C221, C223, C225, C227, C228</t>
+  </si>
+  <si>
+    <t>R114, R116, R117, R121, R124, R127, R133, R135, R140, R143, R148, R200, R202, R204, R205, R207, R208</t>
+  </si>
+  <si>
+    <t>C103, C202, C203, C206, C207, C208, C213, C214, C215, C220, C222, C224, C226, C229, C230, C231</t>
+  </si>
+  <si>
+    <t>JLC Part No</t>
+  </si>
+  <si>
+    <t>C116978</t>
+  </si>
+  <si>
+    <t>C28060</t>
+  </si>
+  <si>
+    <t>C116655</t>
+  </si>
+  <si>
+    <t>C99782</t>
+  </si>
+  <si>
+    <t>C113303</t>
+  </si>
+  <si>
+    <t>C1590</t>
+  </si>
+  <si>
+    <t>C9890</t>
+  </si>
+  <si>
+    <t>MFR Part No</t>
+  </si>
+  <si>
+    <t>C293569</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>MMBT4401(RANGE:100-300)</t>
+  </si>
+  <si>
+    <t>C2144</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>C1592</t>
+  </si>
+  <si>
+    <t>C15850</t>
+  </si>
+  <si>
+    <t>R115, R128, R130, R132, R134, R136, R138, R139, R142, R144, R151
 R146, R147, R149, R150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inductor </t>
-  </si>
-  <si>
-    <t>P-Channel Surface Mount Mosfet</t>
-  </si>
-  <si>
-    <t>Microcontroller</t>
-  </si>
-  <si>
-    <t>5V regulator</t>
-  </si>
-  <si>
-    <t>3.3V regulator</t>
-  </si>
-  <si>
-    <t>GCT_MEM2051</t>
-  </si>
-  <si>
-    <t>VISHAY_SIS468DN-T1</t>
-  </si>
-  <si>
-    <t>MEM2051</t>
-  </si>
-  <si>
-    <t>USB C connector</t>
-  </si>
-  <si>
-    <t>0603</t>
-  </si>
-  <si>
-    <t>0805</t>
-  </si>
-  <si>
-    <t>10VSON</t>
-  </si>
-  <si>
-    <t>CAPACITOR</t>
-  </si>
-  <si>
-    <t>USB ESD</t>
-  </si>
-  <si>
-    <t>RESISTOR</t>
-  </si>
-  <si>
-    <t>Micro SD Card connector</t>
-  </si>
-  <si>
-    <t>C201, C204, C221, C223, C225, C227, C228</t>
-  </si>
-  <si>
-    <t>R114, R116, R117, R121, R124, R127, R133, R135, R140, R143, R148, R200, R202, R204, R205, R207, R208</t>
-  </si>
-  <si>
-    <t>C103, C202, C203, C206, C207, C208, C213, C214, C215, C220, C222, C224, C226, C229, C230, C231</t>
   </si>
 </sst>
 </file>
@@ -701,7 +692,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -710,6 +701,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -772,21 +764,19 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F5A1808-0047-49B1-96DE-517D79516FD0}" name="Table1" displayName="Table1" ref="B1:E16" totalsRowShown="0">
-  <autoFilter ref="B1:E16" xr:uid="{3F5A1808-0047-49B1-96DE-517D79516FD0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E16">
-    <sortCondition descending="1" ref="B1:B16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F5A1808-0047-49B1-96DE-517D79516FD0}" name="Table1" displayName="Table1" ref="B1:G12" totalsRowShown="0">
+  <autoFilter ref="B1:G12" xr:uid="{3F5A1808-0047-49B1-96DE-517D79516FD0}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E12">
+    <sortCondition descending="1" ref="B1:B12"/>
   </sortState>
-  <tableColumns count="4">
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{42B11F5B-A91F-4B42-B4E8-B35F548315DA}" name="Qty"/>
     <tableColumn id="3" xr3:uid="{E6B9FB98-E350-4520-A307-12FD50263B2D}" name="Designator"/>
     <tableColumn id="4" xr3:uid="{1D51CB69-F028-4779-A835-D90473B94B9A}" name="Package" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{84C859D8-B49E-4105-9CEB-B7D2BABAA3EE}" name="Description"/>
+    <tableColumn id="2" xr3:uid="{5FE04A48-52EC-4FF5-A32F-87E897B7DDCA}" name="JLC Part No"/>
+    <tableColumn id="5" xr3:uid="{A8747573-2C37-41FB-BF97-E0CADB90E00F}" name="MFR Part No"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1109,16 +1099,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E12622-1509-4756-8C38-8BF3F9E042CF}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.89453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.68359375" customWidth="1"/>
+    <col min="1" max="1" width="23.5234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.05078125" customWidth="1"/>
     <col min="4" max="4" width="19.68359375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.20703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.26171875" customWidth="1"/>
@@ -1126,15 +1116,15 @@
     <col min="8" max="8" width="2.47265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1142,8 +1132,14 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1151,16 +1147,19 @@
         <v>17</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1168,16 +1167,19 @@
         <v>16</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1185,33 +1187,39 @@
         <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1219,16 +1227,19 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1239,13 +1250,16 @@
         <v>5</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1259,143 +1273,98 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="6">
+        <v>473521001</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>34</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="5">
+        <v>473521001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" t="s">
-        <v>52</v>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C18" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>